<commit_message>
Update New Commodity for Space Heating per BER
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_RSD_UnitBoilers.xlsx
+++ b/SuppXLS/Scen_B_RSD_UnitBoilers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F6E3931-DC4D-407D-8D21-49F785D1CCBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{925474E8-C627-45D6-8753-AB1559323A12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="3" r:id="rId1"/>
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="106">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -485,6 +485,15 @@
   </si>
   <si>
     <t>One heating system is assigned per dwelling ( except Fireplace can be used as secondary space heating)</t>
+  </si>
+  <si>
+    <t>Apt*</t>
+  </si>
+  <si>
+    <t>Att*</t>
+  </si>
+  <si>
+    <t>Det*</t>
   </si>
 </sst>
 </file>
@@ -890,7 +899,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF589795-735D-472B-87C8-FC6EC46E957E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -934,7 +943,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CFC9C4E-989C-415B-9DCC-4D77CA4F61D1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -983,7 +992,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A65AE3C-9B75-4277-A560-96390405CAC1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1033,7 +1042,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{792663B9-3F52-4451-A64A-BE972DFF3965}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1083,7 +1092,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF612F31-0A33-4A64-9B7C-9591CC922F41}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1132,7 +1141,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C2BB85C-7544-4BDA-B015-6140A15ACA95}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
               <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{B1489C0F-1609-4587-A5BA-D0B99739EA08}"/>
@@ -1542,7 +1551,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:Z99"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B21" sqref="B21:D22"/>
     </sheetView>
   </sheetViews>
@@ -5169,8 +5178,8 @@
   </sheetPr>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5178,7 +5187,7 @@
     <col min="1" max="1" width="24.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="64.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" style="2" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" style="2" customWidth="1"/>
     <col min="6" max="6" width="9.7109375" style="2" customWidth="1"/>
     <col min="7" max="10" width="8.42578125" style="2" customWidth="1"/>
@@ -5254,18 +5263,18 @@
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="str">
         <f>"UC_RSD_UnitBoiler_SH-"&amp;L8</f>
-        <v>UC_RSD_UnitBoiler_SH-Apt</v>
+        <v>UC_RSD_UnitBoiler_SH-Apt*</v>
       </c>
       <c r="B8" s="2" t="str">
         <f>"Number of boilers providing space heat equals number of dwellings in RSD "&amp;L8</f>
-        <v>Number of boilers providing space heat equals number of dwellings in RSD Apt</v>
+        <v>Number of boilers providing space heat equals number of dwellings in RSD Apt*</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>85</v>
       </c>
       <c r="D8" s="2" t="str">
         <f>"RSDSH_"&amp;L8</f>
-        <v>RSDSH_Apt</v>
+        <v>RSDSH_Apt*</v>
       </c>
       <c r="E8" s="15" t="s">
         <v>79</v>
@@ -5287,13 +5296,13 @@
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2" t="s">
-        <v>9</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C9" s="2" t="str">
         <f>"R-BLD_"&amp;L8&amp;"*"</f>
-        <v>R-BLD_Apt*</v>
+        <v>R-BLD_Apt**</v>
       </c>
       <c r="H9" s="2">
         <v>-1</v>
@@ -5303,18 +5312,18 @@
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="str">
         <f>"UC_RSD_UnitBoiler_SH-"&amp;L10</f>
-        <v>UC_RSD_UnitBoiler_SH-Att</v>
+        <v>UC_RSD_UnitBoiler_SH-Att*</v>
       </c>
       <c r="B10" s="2" t="str">
         <f>"Number of boilers providing space heat equals number of dwellings in RSD "&amp;L10</f>
-        <v>Number of boilers providing space heat equals number of dwellings in RSD Att</v>
+        <v>Number of boilers providing space heat equals number of dwellings in RSD Att*</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>85</v>
       </c>
       <c r="D10" s="2" t="str">
         <f>"RSDSH_"&amp;L10</f>
-        <v>RSDSH_Att</v>
+        <v>RSDSH_Att*</v>
       </c>
       <c r="E10" s="15" t="s">
         <v>79</v>
@@ -5336,13 +5345,13 @@
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2" t="s">
-        <v>8</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C11" s="2" t="str">
         <f>"R-BLD_"&amp;L10&amp;"*"</f>
-        <v>R-BLD_Att*</v>
+        <v>R-BLD_Att**</v>
       </c>
       <c r="H11" s="2">
         <v>-1</v>
@@ -5352,18 +5361,18 @@
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="str">
         <f>"UC_RSD_UnitBoiler_SH-"&amp;L12</f>
-        <v>UC_RSD_UnitBoiler_SH-Det</v>
+        <v>UC_RSD_UnitBoiler_SH-Det*</v>
       </c>
       <c r="B12" s="2" t="str">
         <f>"Number of boilers providing space heat equals number of dwellings in RSD "&amp;L12</f>
-        <v>Number of boilers providing space heat equals number of dwellings in RSD Det</v>
+        <v>Number of boilers providing space heat equals number of dwellings in RSD Det*</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>85</v>
       </c>
       <c r="D12" s="2" t="str">
         <f>"RSDSH_"&amp;L12</f>
-        <v>RSDSH_Det</v>
+        <v>RSDSH_Det*</v>
       </c>
       <c r="E12" s="15" t="s">
         <v>79</v>
@@ -5385,7 +5394,7 @@
       </c>
       <c r="K12" s="2"/>
       <c r="L12" s="2" t="s">
-        <v>10</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -5393,7 +5402,7 @@
       <c r="B13" s="3"/>
       <c r="C13" s="3" t="str">
         <f>"R-BLD_"&amp;L12&amp;"*"</f>
-        <v>R-BLD_Det*</v>
+        <v>R-BLD_Det**</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>

</xml_diff>

<commit_message>
Make Solar not restricted to buildings and fix electric heating price
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_RSD_UnitBoilers.xlsx
+++ b/SuppXLS/Scen_B_RSD_UnitBoilers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{925474E8-C627-45D6-8753-AB1559323A12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90DC78C9-66E9-4B9C-B79F-AC1CF6D852E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
   </bookViews>
@@ -433,9 +433,6 @@
     <t>R-BLD*</t>
   </si>
   <si>
-    <t>*,-*RTFT*,-R*FPL_N1</t>
-  </si>
-  <si>
     <t>TIMES-Ireland Model</t>
   </si>
   <si>
@@ -494,6 +491,9 @@
   </si>
   <si>
     <t>Det*</t>
+  </si>
+  <si>
+    <t>*,-*RTFT*,-R*FPL_N1,-R*SOL_N1</t>
   </si>
 </sst>
 </file>
@@ -1991,7 +1991,7 @@
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="33" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B16" s="33"/>
       <c r="C16" s="33"/>
@@ -2077,10 +2077,10 @@
     </row>
     <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B19" s="32" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C19" s="32"/>
       <c r="D19" s="32"/>
@@ -2109,10 +2109,10 @@
     </row>
     <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B20" s="32" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C20" s="32"/>
       <c r="D20" s="32"/>
@@ -2141,10 +2141,10 @@
     </row>
     <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B21" s="35" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C21" s="35"/>
       <c r="D21" s="35"/>
@@ -2201,10 +2201,10 @@
     </row>
     <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B23" s="32" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C23" s="32"/>
       <c r="D23" s="32"/>
@@ -2234,7 +2234,7 @@
     <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="24"/>
       <c r="B24" s="32" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C24" s="32"/>
       <c r="D24" s="32"/>
@@ -2291,10 +2291,10 @@
     </row>
     <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B26" s="32" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C26" s="32"/>
       <c r="D26" s="32"/>
@@ -2324,7 +2324,7 @@
     <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="24"/>
       <c r="B27" s="32" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C27" s="32"/>
       <c r="D27" s="32"/>
@@ -2381,7 +2381,7 @@
     </row>
     <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B29" s="28">
         <v>1</v>
@@ -2413,10 +2413,10 @@
     </row>
     <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="B30" s="34" t="s">
         <v>93</v>
-      </c>
-      <c r="B30" s="34" t="s">
-        <v>94</v>
       </c>
       <c r="C30" s="32"/>
       <c r="D30" s="32"/>
@@ -2445,10 +2445,10 @@
     </row>
     <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="B31" s="32" t="s">
         <v>95</v>
-      </c>
-      <c r="B31" s="32" t="s">
-        <v>96</v>
       </c>
       <c r="C31" s="32"/>
       <c r="D31" s="32"/>
@@ -2478,7 +2478,7 @@
     <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="30"/>
       <c r="B32" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C32" s="30"/>
       <c r="D32" s="30"/>
@@ -5179,7 +5179,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5270,7 +5270,7 @@
         <v>Number of boilers providing space heat equals number of dwellings in RSD Apt*</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="D8" s="2" t="str">
         <f>"RSDSH_"&amp;L8</f>
@@ -5296,7 +5296,7 @@
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -5319,7 +5319,7 @@
         <v>Number of boilers providing space heat equals number of dwellings in RSD Att*</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="D10" s="2" t="str">
         <f>"RSDSH_"&amp;L10</f>
@@ -5345,7 +5345,7 @@
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -5368,7 +5368,7 @@
         <v>Number of boilers providing space heat equals number of dwellings in RSD Det*</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="D12" s="2" t="str">
         <f>"RSDSH_"&amp;L12</f>
@@ -5394,7 +5394,7 @@
       </c>
       <c r="K12" s="2"/>
       <c r="L12" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update - Solar UC allowed to have water heater and solar and Heating Profiles and dummies coming in due to fixed share in 2018
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_RSD_UnitBoilers.xlsx
+++ b/SuppXLS/Scen_B_RSD_UnitBoilers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90DC78C9-66E9-4B9C-B79F-AC1CF6D852E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E7241E-12E9-41DD-8A43-7C3BA21CED22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
+    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="3" r:id="rId1"/>
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="107">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -493,7 +493,10 @@
     <t>Det*</t>
   </si>
   <si>
-    <t>*,-*RTFT*,-R*FPL_N1,-R*SOL_N1</t>
+    <t>,-R*SOL_N1</t>
+  </si>
+  <si>
+    <t>,-*RTFT*,-R*FPL_N1</t>
   </si>
 </sst>
 </file>
@@ -5179,7 +5182,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5270,7 +5273,7 @@
         <v>Number of boilers providing space heat equals number of dwellings in RSD Apt*</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D8" s="2" t="str">
         <f>"RSDSH_"&amp;L8</f>
@@ -5319,7 +5322,7 @@
         <v>Number of boilers providing space heat equals number of dwellings in RSD Att*</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D10" s="2" t="str">
         <f>"RSDSH_"&amp;L10</f>
@@ -5368,7 +5371,7 @@
         <v>Number of boilers providing space heat equals number of dwellings in RSD Det*</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D12" s="2" t="str">
         <f>"RSDSH_"&amp;L12</f>
@@ -5425,6 +5428,9 @@
         <f>"Number of boilers providing water heating equals number of dwellings in RSD "&amp;L14</f>
         <v>Number of boilers providing water heating equals number of dwellings in RSD Apt</v>
       </c>
+      <c r="C14" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="D14" s="2" t="str">
         <f>"RSDWH_"&amp;L14</f>
         <v>RSDWH_Apt</v>
@@ -5469,6 +5475,9 @@
         <f>"Number of boiler providing water heatings equals number of dwellings in RSD "&amp;L16</f>
         <v>Number of boiler providing water heatings equals number of dwellings in RSD Att</v>
       </c>
+      <c r="C16" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="D16" s="2" t="str">
         <f>"RSDWH_"&amp;L16</f>
         <v>RSDWH_Att</v>
@@ -5512,6 +5521,9 @@
       <c r="B18" s="2" t="str">
         <f>"Number of boilers providing water heating equals number of dwellings in RSD "&amp;L18</f>
         <v>Number of boilers providing water heating equals number of dwellings in RSD Det</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="D18" s="2" t="str">
         <f>"RSDWH_"&amp;L18</f>

</xml_diff>

<commit_message>
"E-LM" change to "IE-LM" for regions
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_RSD_UnitBoilers.xlsx
+++ b/SuppXLS/Scen_B_RSD_UnitBoilers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E7241E-12E9-41DD-8A43-7C3BA21CED22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0391FB7-9362-4004-88A0-D325DE2415DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="3" r:id="rId1"/>
@@ -493,10 +493,10 @@
     <t>Det*</t>
   </si>
   <si>
-    <t>,-R*SOL_N1</t>
-  </si>
-  <si>
     <t>,-*RTFT*,-R*FPL_N1</t>
+  </si>
+  <si>
+    <t>,-R*SOL*</t>
   </si>
 </sst>
 </file>
@@ -5182,7 +5182,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5273,7 +5273,7 @@
         <v>Number of boilers providing space heat equals number of dwellings in RSD Apt*</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D8" s="2" t="str">
         <f>"RSDSH_"&amp;L8</f>
@@ -5322,7 +5322,7 @@
         <v>Number of boilers providing space heat equals number of dwellings in RSD Att*</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D10" s="2" t="str">
         <f>"RSDSH_"&amp;L10</f>
@@ -5371,7 +5371,7 @@
         <v>Number of boilers providing space heat equals number of dwellings in RSD Det*</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D12" s="2" t="str">
         <f>"RSDSH_"&amp;L12</f>
@@ -5429,7 +5429,7 @@
         <v>Number of boilers providing water heating equals number of dwellings in RSD Apt</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D14" s="2" t="str">
         <f>"RSDWH_"&amp;L14</f>
@@ -5476,7 +5476,7 @@
         <v>Number of boiler providing water heatings equals number of dwellings in RSD Att</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D16" s="2" t="str">
         <f>"RSDWH_"&amp;L16</f>
@@ -5523,7 +5523,7 @@
         <v>Number of boilers providing water heating equals number of dwellings in RSD Det</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D18" s="2" t="str">
         <f>"RSDWH_"&amp;L18</f>

</xml_diff>

<commit_message>
Unit Boiler UC apply per region
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_RSD_UnitBoilers.xlsx
+++ b/SuppXLS/Scen_B_RSD_UnitBoilers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0391FB7-9362-4004-88A0-D325DE2415DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{066FC01C-6705-4867-954D-7EEB201586E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
   </bookViews>
@@ -5182,7 +5182,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5210,8 +5210,8 @@
     </row>
     <row r="4" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,"~UC_Sets: R_E:",_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,"")))</f>
-        <v>~UC_Sets: R_E: IE,National</v>
+        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:'Regions'!$AD$3)</f>
+        <v>IE,National,IE-CW,IE-D,IE-KE,IE-KK,IE-LS,IE-LD,IE-LH,IE-MH,IE-OY,IE-WH,IE-WX,IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
       </c>
       <c r="K4" s="2"/>
     </row>

</xml_diff>

<commit_message>
Update DH sector UC
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_RSD_UnitBoilers.xlsx
+++ b/SuppXLS/Scen_B_RSD_UnitBoilers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{066FC01C-6705-4867-954D-7EEB201586E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79DC7B13-F465-4F76-87F0-34C0A463ADD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
   </bookViews>
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="119">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -498,6 +498,42 @@
   <si>
     <t>,-R*SOL*</t>
   </si>
+  <si>
+    <t>SRVHET</t>
+  </si>
+  <si>
+    <t>*HET_C</t>
+  </si>
+  <si>
+    <t>Share of sector heating served by district heating in City</t>
+  </si>
+  <si>
+    <t>FT-RSDHET_C</t>
+  </si>
+  <si>
+    <t>UC_DH_Share_C</t>
+  </si>
+  <si>
+    <t>UC_RHSRTS</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Cset_CN</t>
+  </si>
+  <si>
+    <t>Pset_CO</t>
+  </si>
+  <si>
+    <t>Pset_CI</t>
+  </si>
+  <si>
+    <t>Pset_PN</t>
+  </si>
+  <si>
+    <t>Pset_Set</t>
+  </si>
 </sst>
 </file>
 
@@ -506,7 +542,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -632,8 +668,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -673,6 +715,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="51"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -762,7 +816,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -858,6 +912,12 @@
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink 2" xfId="3" xr:uid="{BB0011A7-1A39-491F-B9B7-C0D5F250487E}"/>
@@ -5179,10 +5239,10 @@
   <sheetPr codeName="Sheet2">
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5656,6 +5716,121 @@
         <v>-1</v>
       </c>
     </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A30" s="8"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A31" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="C31" s="41" t="s">
+        <v>117</v>
+      </c>
+      <c r="D31" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="E31" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="F31" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="G31" s="40" t="s">
+        <v>113</v>
+      </c>
+      <c r="H31" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="I31" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="J31" s="40" t="s">
+        <v>112</v>
+      </c>
+      <c r="K31" s="39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A32" s="38" t="s">
+        <v>111</v>
+      </c>
+      <c r="B32" s="8"/>
+      <c r="C32" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8">
+        <v>2019</v>
+      </c>
+      <c r="H32" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="I32" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="J32" s="8"/>
+      <c r="K32" s="38" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" s="8"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="D33" s="8"/>
+      <c r="E33" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8">
+        <v>2019</v>
+      </c>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8">
+        <v>1</v>
+      </c>
+      <c r="J33" s="8"/>
+      <c r="K33" s="8"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" s="8"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="36"/>
+      <c r="D34" s="36"/>
+      <c r="E34" s="36"/>
+      <c r="F34" s="36"/>
+      <c r="G34" s="36">
+        <v>0</v>
+      </c>
+      <c r="H34" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="I34" s="36"/>
+      <c r="J34" s="36">
+        <v>5</v>
+      </c>
+      <c r="K34" s="36"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>